<commit_message>
Update is_positive field translations to English in JSON to Excel converter
</commit_message>
<xml_diff>
--- a/keyword_report.xlsx
+++ b/keyword_report.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -519,7 +519,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -544,7 +544,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -669,7 +669,7 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -719,7 +719,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -769,7 +769,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -819,7 +819,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -844,7 +844,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -894,7 +894,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
@@ -1299,7 +1299,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1424,7 +1424,7 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -1574,7 +1574,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1749,7 +1749,7 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2224,7 +2224,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D44" s="2" t="inlineStr">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -2679,7 +2679,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -2854,7 +2854,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -2879,7 +2879,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
@@ -2979,7 +2979,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -3079,7 +3079,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
@@ -3154,7 +3154,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
@@ -3379,7 +3379,7 @@
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
@@ -3429,7 +3429,7 @@
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
@@ -3454,7 +3454,7 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
@@ -3554,7 +3554,7 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -3579,7 +3579,7 @@
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D42" s="2" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr">
@@ -3654,7 +3654,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3679,7 +3679,7 @@
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3754,7 +3754,7 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr">
@@ -3804,7 +3804,7 @@
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D50" s="2" t="inlineStr">
@@ -3829,7 +3829,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr">
@@ -3904,7 +3904,7 @@
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
@@ -3929,7 +3929,7 @@
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
@@ -3954,7 +3954,7 @@
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
@@ -3979,7 +3979,7 @@
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
@@ -4029,7 +4029,7 @@
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr">
@@ -4104,7 +4104,7 @@
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D62" s="2" t="inlineStr">
@@ -4129,7 +4129,7 @@
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D67" s="2" t="inlineStr">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D69" s="2" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D71" s="2" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr">
@@ -4379,7 +4379,7 @@
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D73" s="2" t="inlineStr">
@@ -4404,7 +4404,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -4454,7 +4454,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -4479,7 +4479,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -4504,7 +4504,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -4529,7 +4529,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -4554,7 +4554,7 @@
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr">
@@ -4579,7 +4579,7 @@
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D81" s="2" t="inlineStr">
@@ -4604,7 +4604,7 @@
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
@@ -4629,7 +4629,7 @@
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D83" s="2" t="inlineStr">
@@ -4654,7 +4654,7 @@
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D84" s="2" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D85" s="2" t="inlineStr">
@@ -4704,7 +4704,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D87" s="2" t="inlineStr">
@@ -4754,7 +4754,7 @@
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr">
@@ -4779,7 +4779,7 @@
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D89" s="2" t="inlineStr">
@@ -4804,7 +4804,7 @@
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr">
@@ -4829,7 +4829,7 @@
       </c>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D91" s="2" t="inlineStr">
@@ -4854,7 +4854,7 @@
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr">
@@ -4879,7 +4879,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D93" s="2" t="inlineStr">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D95" s="2" t="inlineStr">
@@ -4954,7 +4954,7 @@
       </c>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D96" s="2" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D97" s="2" t="inlineStr">
@@ -5004,7 +5004,7 @@
       </c>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D98" s="2" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="C99" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D99" s="2" t="inlineStr">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D100" s="2" t="inlineStr">
@@ -5079,7 +5079,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -5159,7 +5159,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -5184,7 +5184,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -5209,7 +5209,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -5234,7 +5234,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -5259,7 +5259,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -5284,7 +5284,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -5334,7 +5334,7 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -5384,7 +5384,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -5434,7 +5434,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
@@ -5459,7 +5459,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -5484,7 +5484,7 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
@@ -5509,7 +5509,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -5559,7 +5559,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -5584,7 +5584,7 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -5634,7 +5634,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
@@ -5659,7 +5659,7 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -5684,7 +5684,7 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
@@ -5734,7 +5734,7 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
@@ -5759,7 +5759,7 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
@@ -5784,7 +5784,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -5809,7 +5809,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -5834,7 +5834,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -5859,7 +5859,7 @@
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
@@ -5909,7 +5909,7 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -5959,7 +5959,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -5984,7 +5984,7 @@
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
@@ -6009,7 +6009,7 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
@@ -6034,7 +6034,7 @@
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
@@ -6084,7 +6084,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
@@ -6109,7 +6109,7 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D42" s="2" t="inlineStr">
@@ -6184,7 +6184,7 @@
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr">
@@ -6209,7 +6209,7 @@
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D44" s="2" t="inlineStr">
@@ -6234,7 +6234,7 @@
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
@@ -6259,7 +6259,7 @@
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
@@ -6284,7 +6284,7 @@
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr">
@@ -6359,7 +6359,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -6384,7 +6384,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
@@ -6409,7 +6409,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
@@ -6434,7 +6434,7 @@
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr">
@@ -6459,7 +6459,7 @@
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
@@ -6484,7 +6484,7 @@
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
@@ -6509,7 +6509,7 @@
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
@@ -6534,7 +6534,7 @@
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
@@ -6559,7 +6559,7 @@
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
@@ -6584,7 +6584,7 @@
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr">
@@ -6634,7 +6634,7 @@
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr">
@@ -6659,7 +6659,7 @@
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D62" s="2" t="inlineStr">
@@ -6684,7 +6684,7 @@
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr">
@@ -6734,7 +6734,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr">
@@ -6759,7 +6759,7 @@
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr">
@@ -6784,7 +6784,7 @@
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D67" s="2" t="inlineStr">
@@ -6809,7 +6809,7 @@
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D68" s="2" t="inlineStr">
@@ -6834,7 +6834,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D69" s="2" t="inlineStr">
@@ -6859,7 +6859,7 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
@@ -6884,7 +6884,7 @@
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D71" s="2" t="inlineStr">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr">
@@ -6934,7 +6934,7 @@
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D73" s="2" t="inlineStr">
@@ -6959,7 +6959,7 @@
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr">
@@ -6984,7 +6984,7 @@
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr">
@@ -7009,7 +7009,7 @@
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D76" s="2" t="inlineStr">
@@ -7034,7 +7034,7 @@
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D77" s="2" t="inlineStr">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D79" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr">
@@ -7134,7 +7134,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -7159,7 +7159,7 @@
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
@@ -7184,7 +7184,7 @@
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D83" s="2" t="inlineStr">
@@ -7209,7 +7209,7 @@
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D84" s="2" t="inlineStr">
@@ -7234,7 +7234,7 @@
       </c>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D85" s="2" t="inlineStr">
@@ -7259,7 +7259,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -7284,7 +7284,7 @@
       </c>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D87" s="2" t="inlineStr">
@@ -7309,7 +7309,7 @@
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr">
@@ -7334,7 +7334,7 @@
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D89" s="2" t="inlineStr">
@@ -7359,7 +7359,7 @@
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr">
@@ -7384,7 +7384,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -7409,7 +7409,7 @@
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr">
@@ -7434,7 +7434,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D93" s="2" t="inlineStr">
@@ -7459,7 +7459,7 @@
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr">
@@ -7484,7 +7484,7 @@
       </c>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D95" s="2" t="inlineStr">
@@ -7509,7 +7509,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -7534,7 +7534,7 @@
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D97" s="2" t="inlineStr">
@@ -7559,7 +7559,7 @@
       </c>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D98" s="2" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="C99" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D99" s="2" t="inlineStr">
@@ -7609,7 +7609,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -7634,7 +7634,7 @@
       </c>
       <c r="C101" s="2" t="inlineStr">
         <is>
-          <t>Hayır</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D101" s="2" t="inlineStr">

</xml_diff>